<commit_message>
update template excel export
</commit_message>
<xml_diff>
--- a/public/template/Excel/template01.xlsx
+++ b/public/template/Excel/template01.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Module03_Old\public\template\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\03\public\template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1746CF-FD81-439B-830A-814B4D2B63D1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759C3EC8-CBD8-465A-9C74-2A2D7A0C5F39}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16244,8 +16244,8 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0" header="0.19685039370078741" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F &amp; 　　 &amp;A</oddHeader>
   </headerFooter>
@@ -23859,8 +23859,8 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0" header="0.19685039370078741" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F &amp; 　　 &amp;A</oddHeader>
   </headerFooter>
@@ -31483,8 +31483,8 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0" header="0.19685039370078741" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="75" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F &amp; 　　 &amp;A</oddHeader>
   </headerFooter>
@@ -46663,8 +46663,8 @@
   </mergeCells>
   <phoneticPr fontId="2"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0" header="0.19685039370078741" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;F &amp; 　　 &amp;A</oddHeader>
   </headerFooter>

</xml_diff>